<commit_message>
update prepare merge to dev
</commit_message>
<xml_diff>
--- a/MyKitchen/_ADocumentation/Development_Matrix.xlsx
+++ b/MyKitchen/_ADocumentation/Development_Matrix.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\source\repos\MyKitchen\MyKitchen\_ADocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C032F50-E4BC-47A8-BD8B-22FE71B5333B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176DFA83-506E-4275-A32C-1BCECA756B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="11423" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Epics" sheetId="4" r:id="rId1"/>
     <sheet name="Tasks" sheetId="1" r:id="rId2"/>
-    <sheet name="Tests" sheetId="2" r:id="rId3"/>
-    <sheet name="Ideas" sheetId="3" r:id="rId4"/>
+    <sheet name="Notes" sheetId="6" r:id="rId3"/>
+    <sheet name="Bugs" sheetId="5" r:id="rId4"/>
+    <sheet name="Tests" sheetId="2" r:id="rId5"/>
+    <sheet name="Ideas" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -80,9 +82,6 @@
     <t>add sorting to food items</t>
   </si>
   <si>
-    <t>MEALS SHOW ALL ITEMS in the GRID!!! - see if we implement this using a selectmany!!! If YES, blog about this! This is the next step of our process.!</t>
-  </si>
-  <si>
     <t>need to add userid to dbo.meals table</t>
   </si>
   <si>
@@ -104,17 +103,86 @@
     <t>food items should require name</t>
   </si>
   <si>
-    <t>remove cost</t>
-  </si>
-  <si>
     <t>add star ratings - how much do I enjoy eating this food</t>
+  </si>
+  <si>
+    <t>create a way to delete everything in the database - and seed users with fresh data</t>
+  </si>
+  <si>
+    <t>create a logo for each of the food groups to better visualize WTF Is happening within the meal builder</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>User Accounts</t>
+  </si>
+  <si>
+    <t>Food Items Grid</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Meals Grid</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>create thumbnail images for each of the food groups</t>
+  </si>
+  <si>
+    <t>set cost as low , medium, high</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">6/14/2020
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I need to get a V1 up online soon - let's finish the iteration 1 tasks, create the basic product info on IH, and start sharing some of our information on the blueprogrammer blog.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,13 +197,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,14 +235,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -168,6 +262,41 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8CAD22FF-6E79-47BF-A178-ED880616A7D3}" name="Table2" displayName="Table2" ref="A1:C38" totalsRowShown="0">
+  <autoFilter ref="A1:C38" xr:uid="{13508EEF-1008-4DAF-9731-2330DBA6E745}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{25DF893B-E007-46AF-B6F7-84BE7A1FE3E4}" name="Description"/>
+    <tableColumn id="2" xr3:uid="{234C1BEA-95B9-4679-B638-37D8112B73D8}" name="Status"/>
+    <tableColumn id="3" xr3:uid="{2FC6F8A7-E0B6-48E0-8930-5ACD861F868D}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85CBF929-9E80-4092-ACCD-91EC86E2BD12}" name="Table1" displayName="Table1" ref="A1:E35" totalsRowShown="0">
+  <autoFilter ref="A1:E35" xr:uid="{0FB0A204-BD9D-455A-B6D7-9170A75F330D}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
+    <sortCondition ref="C1:C35"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E8228895-ADB7-4953-A0AC-3D7C0E8DD204}" name="Description"/>
+    <tableColumn id="5" xr3:uid="{8F42B2B1-74EF-404F-8583-858D2AD2058D}" name="Iteration"/>
+    <tableColumn id="2" xr3:uid="{7CCEF032-564F-49B7-8979-EAD1517702C3}" name="Area"/>
+    <tableColumn id="3" xr3:uid="{DD010FE9-0774-4777-8F3D-FBAB176B6F07}" name="Status"/>
+    <tableColumn id="4" xr3:uid="{22EEF08E-D724-42BA-9811-031DF524A0BA}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,122 +562,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313B1285-A7F1-4F27-A3D5-6AFF284C9D38}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D6" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="48.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="117.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.86328125" customWidth="1"/>
+    <col min="3" max="3" width="37.1328125" customWidth="1"/>
+    <col min="4" max="4" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="17" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="18" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="19" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="20" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="22" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="23" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="24" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="25" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="26" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="27" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="28" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="29" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="30" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="31" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="32" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="33" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="34" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="35" hidden="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0763DA47-DA04-40A0-ADB5-D092D84E77C4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="47.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="384.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -557,12 +848,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05399C00-933D-435F-A97E-86CAD5CDE81C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE53BFD-BC1F-4C97-AF05-864BBA9154A8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -604,12 +907,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C95EB6-97DD-4B8D-BD89-BE7B160B8B3C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -627,6 +930,11 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>